<commit_message>
1. Developed a new test in catalog module - VerifyReq_SearchRejectedOrders. 2. Added the following methods in Recent Order Information page:   a.getCart_RejectedOrders();   b.getRFQ_RejectedOrders();   c.getREQ_RejectedOrders(); and   d.enterSearchCriteriaAndVerifyRejectedOrders().
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyCatalogSearch.xlsx
+++ b/src/test/resources/datasheets/VerifyCatalogSearch.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="6210"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -387,7 +386,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Moved Test Files to new Package "SearchFunctionalty"
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyCatalogSearch.xlsx
+++ b/src/test/resources/datasheets/VerifyCatalogSearch.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15435" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="VerifyCatalogSearch" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -42,9 +43,6 @@
     <t>MAGNA DECOPLAS</t>
   </si>
   <si>
-    <t>COMPUTER DESKTOP</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
@@ -52,6 +50,9 @@
   </si>
   <si>
     <t>bpo</t>
+  </si>
+  <si>
+    <t>DESKTOPs</t>
   </si>
 </sst>
 </file>
@@ -386,7 +387,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -419,16 +420,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>